<commit_message>
test login multi account tiktok
</commit_message>
<xml_diff>
--- a/TiktokAcount.xlsx
+++ b/TiktokAcount.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{622692CE-ADC3-49D1-93E2-6AAE6B0C66E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75DA3CFD-8ED6-4455-A554-0F7EDEE2526A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="1665" windowWidth="24345" windowHeight="13815" xr2:uid="{417DF7B6-A403-47CD-B886-1559DD8E10A2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
   <si>
     <t>user6881719028025</t>
   </si>
@@ -425,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EBB6772-9F5E-4DC1-8233-19710F297856}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,6 +461,30 @@
         <v>5</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>